<commit_message>
try Ragas and add new test-questions
</commit_message>
<xml_diff>
--- a/wq.xlsx
+++ b/wq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zirong/Desktop/CCD_RAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC007F6-5FBE-FA4E-A437-A5699BE38774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD998CA7-D28A-1B47-83AB-585B8E34AB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="23760" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="240" yWindow="740" windowWidth="23760" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -246,9 +246,6 @@
     <t>「麻黃附子細辛湯」為治療風寒表證兼陽虛自汗之常用方。</t>
   </si>
   <si>
-    <t>犬貓熱性腹瀉屬濕熱時，常選用「白頭翁湯」。</t>
-  </si>
-  <si>
     <t>GB-34 陽陵泉為筋腱之會，常治後肢跛行及韌帶損傷。</t>
   </si>
   <si>
@@ -516,24 +513,6 @@
   </si>
   <si>
     <t>判斷依據：
-* 麻黃附子細辛湯是一種中醫方劑，主要用於治療風寒表證兼陽虛自汗。
-* LI-11曲池是指中醫學中的穴位之一，位於前肢外側的肘橫紋外側終點。
-* LU-1中府、LU-5尺澤和LI-10前理也是中醫學中的穴位，但不是麻黃附子細辛湯治療風寒表證兼陽虛自汗的主要相關穴位。
-結論：False</t>
-  </si>
-  <si>
-    <t>判斷依據：
-1. 《中藥學》教科書中提到，犬貓熱性腹瀉屬濕熱時，常選用「白頭翁湯」，但沒有明確指出該湯的組成和作用機制。
-2. 中醫理論中，白頭翁湯主要用于治療濕熱病症，如腸躁痢疾、腹瀉等，但也需要根據個體情況進行調整。
-結論：False
-原因：犬貓熱性腹瀉屬濕熱時，並不是常選用「白頭翁湯」。中醫理論中，白頭翁湯主要用于治療濕熱病症，如腸躁痢疾、腹瀉等，但也需要根據個體情況進行調整。
-參考來源：
-* 《中藥學》教科書
-* 中醫理論
-備註：本答案僅基於提供的文獻內容進行回答，若有更詳細或相關資訊可供參考。</t>
-  </si>
-  <si>
-    <t>判斷依據：
 * GB-34 陽陵泉的定位和功能
 * LI-10 前理的定位和功能
 * LI-11 曲池的定位和功能
@@ -559,14 +538,6 @@
 2. 中醫理論和實踐中的耳炎和聽力退化的治療方法。
 根據《針灸大全》的描述，LI-11曲池主要用於治療風熱、免疫相關疾病、咽炎、牙痛等，而非耳炎或聽力退化。益氣聰明湯中通常使用黃芪作為君藥，但是該湯方和針灸點位不一定直接相關。
 結論：False</t>
-  </si>
-  <si>
-    <t>判斷依據：
-1. 《中醫藥學》教材中的相關內容
-2. 中醫藥典故中黃連的特性和用途
-3. 熱毒血熱性皮膚病的病理機制
-根據上述來源和知識，我們可以得出以下結論：
-結論：True</t>
   </si>
   <si>
     <t>True</t>
@@ -984,6 +955,39 @@
   <si>
     <t>針刺 HT-1 極泉主要治療的是牙痛和口腔炎等問題。根據中醫理論，HT-1 極泉的位置在頭部，是一個重要的穴位，可以用來調節身體的氣血和疏通經絡。
 參考資料：(文獻) Canine Cognitive Dysfunction Pathophysiology Diagnosis and Treatment.pdf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>判斷依據：
+* 麻黃附子細辛湯是一種中醫方劑，主要用於治療風寒表證兼陽虛自汗。
+* LI-11曲池是指中醫學中的穴位之一，位於前肢外側的肘橫紋外側終點。
+* LU-1中府、LU-5尺澤和LI-10前理也是中醫學中的穴位，但不是麻黃附子細辛湯治療風寒表證兼陽虛自汗的主要相關穴位。
+結論：False</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>判斷依據：
+1. 《中藥學》教科書中提到，犬貓熱性腹瀉屬濕熱時，常選用「白頭翁湯」，但沒有明確指出該湯的組成和作用機制。
+2. 中醫理論中，白頭翁湯主要用于治療濕熱病症，如腸躁痢疾、腹瀉等，但也需要根據個體情況進行調整。
+結論：False
+原因：犬貓熱性腹瀉屬濕熱時，並不是常選用「白頭翁湯」。中醫理論中，白頭翁湯主要用于治療濕熱病症，如腸躁痢疾、腹瀉等，但也需要根據個體情況進行調整。
+參考來源：
+* 《中藥學》教科書
+* 中醫理論
+備註：本答案僅基於提供的文獻內容進行回答，若有更詳細或相關資訊可供參考。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>犬貓熱性腹瀉屬濕熱時，常選用「白頭翁湯」。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>判斷依據：
+1. 《中醫藥學》教材中的相關內容
+2. 中醫藥典故中黃連的特性和用途
+3. 熱毒血熱性皮膚病的病理機制
+根據上述來源和知識，我們可以得出以下結論：
+結論：True</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1396,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:XFD67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1451,13 +1455,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -1477,13 +1481,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
@@ -1497,16 +1501,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H4" s="3">
         <v>0</v>
@@ -1523,16 +1527,16 @@
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
@@ -1549,13 +1553,13 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H6" s="3">
         <v>0</v>
@@ -1572,13 +1576,13 @@
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -1592,16 +1596,16 @@
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
@@ -1615,16 +1619,16 @@
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H9" s="3">
         <v>0</v>
@@ -1638,16 +1642,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H10" s="3">
         <v>0</v>
@@ -1664,13 +1668,13 @@
         <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H11" s="3">
         <v>0</v>
@@ -1684,16 +1688,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H12" s="3">
         <v>0</v>
@@ -1710,13 +1714,13 @@
         <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -1733,13 +1737,13 @@
         <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H14" s="3">
         <v>0</v>
@@ -1756,13 +1760,13 @@
         <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H15" s="3">
         <v>0</v>
@@ -1779,13 +1783,13 @@
         <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H16" s="3">
         <v>0</v>
@@ -1805,13 +1809,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H17" s="3">
         <v>0</v>
@@ -1825,19 +1829,19 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
@@ -1854,13 +1858,13 @@
         <v>21</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H19" s="3">
         <v>0</v>
@@ -1874,19 +1878,19 @@
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -1903,13 +1907,13 @@
         <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H21" s="3">
         <v>0</v>
@@ -1923,19 +1927,19 @@
         <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
@@ -1949,16 +1953,16 @@
         <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
@@ -1975,13 +1979,13 @@
         <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
@@ -1998,13 +2002,13 @@
         <v>24</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H25" s="3">
         <v>0</v>
@@ -2018,16 +2022,16 @@
         <v>9</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
@@ -2044,13 +2048,13 @@
         <v>25</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H27" s="3">
         <v>0</v>
@@ -2070,13 +2074,13 @@
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
@@ -2093,13 +2097,13 @@
         <v>27</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H29" s="2">
         <v>0</v>
@@ -2116,13 +2120,13 @@
         <v>28</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H30" s="3">
         <v>0</v>
@@ -2139,13 +2143,13 @@
         <v>29</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H31" s="2">
         <v>0</v>
@@ -2162,13 +2166,13 @@
         <v>30</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H32" s="2">
         <v>0</v>
@@ -2185,13 +2189,13 @@
         <v>31</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H33" s="3">
         <v>0</v>
@@ -2208,13 +2212,13 @@
         <v>32</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
@@ -2231,13 +2235,13 @@
         <v>33</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
@@ -2254,13 +2258,13 @@
         <v>34</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
@@ -2277,13 +2281,13 @@
         <v>35</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H37" s="3">
         <v>0</v>
@@ -2300,13 +2304,13 @@
         <v>36</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H38" s="3">
         <v>0</v>
@@ -2323,13 +2327,13 @@
         <v>37</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H39" s="2">
         <v>0</v>
@@ -2346,13 +2350,13 @@
         <v>38</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H40" s="2">
         <v>0</v>
@@ -2369,13 +2373,13 @@
         <v>39</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H41" s="3">
         <v>0</v>
@@ -2392,13 +2396,13 @@
         <v>40</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H42" s="3">
         <v>0</v>
@@ -2415,16 +2419,16 @@
         <v>41</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
@@ -2441,13 +2445,13 @@
         <v>42</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H44" s="2">
         <v>0</v>
@@ -2464,13 +2468,13 @@
         <v>43</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H45" s="3">
         <v>0</v>
@@ -2487,107 +2491,107 @@
         <v>44</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="3" customFormat="1" ht="195">
+      <c r="A47" s="3">
+        <v>89</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H46" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="195">
-      <c r="A47" s="2">
-        <v>89</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F47" s="2" t="s">
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="3" customFormat="1" ht="135">
+      <c r="A48" s="3">
+        <v>90</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H47" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="135">
-      <c r="A48" s="2">
-        <v>90</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="3" customFormat="1" ht="150">
+      <c r="A49" s="3">
+        <v>91</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H48" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="150">
-      <c r="A49" s="2">
-        <v>91</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F49" s="2" t="s">
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="3" customFormat="1" ht="120">
+      <c r="A50" s="3">
+        <v>92</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H49" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="120">
-      <c r="A50" s="2">
-        <v>92</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H50" s="2">
+      <c r="H50" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2602,13 +2606,13 @@
         <v>49</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H51" s="2">
         <v>0</v>
@@ -2625,13 +2629,13 @@
         <v>50</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H52" s="2">
         <v>0</v>
@@ -2648,64 +2652,64 @@
         <v>51</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F53" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="3" customFormat="1" ht="180">
+      <c r="A54" s="3">
+        <v>96</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H53" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="180">
-      <c r="A54" s="2">
-        <v>96</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F54" s="2" t="s">
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="3" customFormat="1" ht="210">
+      <c r="A55" s="3">
+        <v>98</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H54" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="210">
-      <c r="A55" s="2">
-        <v>98</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H55" s="2">
+      <c r="G55" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H55" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2723,13 +2727,13 @@
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
@@ -2749,13 +2753,13 @@
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H57" s="2">
         <v>0</v>
@@ -2775,13 +2779,13 @@
         <v>1</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H58" s="2">
         <v>0</v>
@@ -2801,13 +2805,13 @@
         <v>1</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H59" s="2">
         <v>0</v>
@@ -2827,13 +2831,13 @@
         <v>1</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H60" s="2">
         <v>0</v>
@@ -2853,19 +2857,19 @@
         <v>1</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H61" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="165">
+    <row r="62" spans="1:8" ht="120">
       <c r="A62" s="2">
         <v>110</v>
       </c>
@@ -2879,19 +2883,19 @@
         <v>1</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H62" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="342">
+    <row r="63" spans="1:8" ht="270">
       <c r="A63" s="2">
         <v>111</v>
       </c>
@@ -2899,19 +2903,19 @@
         <v>8</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>61</v>
+        <v>149</v>
       </c>
       <c r="D63" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H63" s="2">
         <v>0</v>
@@ -2925,19 +2929,19 @@
         <v>8</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D64" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H64" s="2">
         <v>0</v>
@@ -2951,19 +2955,19 @@
         <v>8</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D65" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F65" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="H65" s="2">
         <v>0</v>
@@ -2977,19 +2981,19 @@
         <v>8</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D66" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H66" s="2">
         <v>0</v>
@@ -3003,19 +3007,19 @@
         <v>8</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H67" s="2">
         <v>0</v>

</xml_diff>